<commit_message>
Ref kredbestandstat pd standard: append -> concat
</commit_message>
<xml_diff>
--- a/hhdaten/grunddaten.xlsx
+++ b/hhdaten/grunddaten.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="619">
   <si>
     <t>gdenr</t>
   </si>
@@ -5226,7 +5226,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5271,8 +5271,8 @@
         <f>F2+G2</f>
         <v>15522.66</v>
       </c>
-      <c r="E2" s="33" t="s">
-        <v>584</v>
+      <c r="E2" s="33">
+        <v>0</v>
       </c>
       <c r="F2" s="33">
         <v>0</v>

</xml_diff>